<commit_message>
all views except change user details is complete
</commit_message>
<xml_diff>
--- a/Camping2000/ProjectFiles/Timeplan.xlsx
+++ b/Camping2000/ProjectFiles/Timeplan.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20311"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deltagare\source\repos\Camping2000\Camping2000\ProjectFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deltagare\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FFC78F8-48E7-43A6-9CDA-097B1D52A634}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179016"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,8 +24,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gästanvändare</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{8AE07757-9250-4135-B051-6BB6C3B74868}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">The following prios are availabe(in decending order):
+CF=Core Feature
+RF=Required Feature
+AF=Add On Feature
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+  <si>
+    <t>cr = Create</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
   <si>
     <t>Activity</t>
   </si>
@@ -32,71 +67,158 @@
     <t>Prio</t>
   </si>
   <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>Create login View</t>
-  </si>
-  <si>
-    <t>create registration view</t>
-  </si>
-  <si>
-    <t>Create overview of Items to book</t>
-  </si>
-  <si>
-    <t>create booking view</t>
-  </si>
-  <si>
-    <t>create confirmation of booking</t>
-  </si>
-  <si>
-    <t>create checkin view</t>
-  </si>
-  <si>
-    <t>create checkin confirmation</t>
-  </si>
-  <si>
-    <t>create checkout view</t>
-  </si>
-  <si>
-    <t>create checkout confirmation</t>
-  </si>
-  <si>
-    <t>create change booking page</t>
-  </si>
-  <si>
-    <t>create change booking confirmation</t>
-  </si>
-  <si>
-    <t>create change guest details view</t>
-  </si>
-  <si>
-    <t>create change guest details confirmation</t>
-  </si>
-  <si>
-    <t>create logout page</t>
-  </si>
-  <si>
-    <t>create registration method</t>
-  </si>
-  <si>
-    <t>Create database</t>
-  </si>
-  <si>
-    <t>create code first classes</t>
-  </si>
-  <si>
-    <t>create log in method</t>
-  </si>
-  <si>
-    <t>create booking method</t>
+    <t xml:space="preserve">cr. Index view </t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>cr. login View</t>
+  </si>
+  <si>
+    <t>cr. registration view</t>
+  </si>
+  <si>
+    <t>cr. overview of Items to book</t>
+  </si>
+  <si>
+    <t>cr. booking view</t>
+  </si>
+  <si>
+    <t>cr. confirmation of booking</t>
+  </si>
+  <si>
+    <t>cr. checkin view</t>
+  </si>
+  <si>
+    <t>cr. checkin confirmation</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>cr. checkout view</t>
+  </si>
+  <si>
+    <t>cr. checkout confirmation</t>
+  </si>
+  <si>
+    <t>cr. view of daily Arrivals/departures</t>
+  </si>
+  <si>
+    <t>cr. change booking page</t>
+  </si>
+  <si>
+    <t>cr. change booking confirmation</t>
+  </si>
+  <si>
+    <t>cr. change guest details view</t>
+  </si>
+  <si>
+    <t>cr. change guest details confirmation</t>
+  </si>
+  <si>
+    <t>cr. logout View</t>
+  </si>
+  <si>
+    <t>cr. code first classes</t>
+  </si>
+  <si>
+    <t>cr. database</t>
+  </si>
+  <si>
+    <t>cr. registration method</t>
+  </si>
+  <si>
+    <t>cr. log in method</t>
+  </si>
+  <si>
+    <t>cr. logout method</t>
+  </si>
+  <si>
+    <t>cr. booking method</t>
+  </si>
+  <si>
+    <t>cr. check in method</t>
+  </si>
+  <si>
+    <t>cr. check out method</t>
+  </si>
+  <si>
+    <t>cr. modify booking method</t>
+  </si>
+  <si>
+    <t>cr. modify guest details method</t>
+  </si>
+  <si>
+    <t>cr. Printout view</t>
+  </si>
+  <si>
+    <t>cr. Printout Controller</t>
+  </si>
+  <si>
+    <t>cr. class for cabin </t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>cr. booking view for cabin</t>
+  </si>
+  <si>
+    <t>cr. confirmation view for cabin</t>
+  </si>
+  <si>
+    <t>cr. controller for cabin</t>
+  </si>
+  <si>
+    <t>cr. class for canoe</t>
+  </si>
+  <si>
+    <t>cr. booking view for canoe</t>
+  </si>
+  <si>
+    <t>cr. confirmation view for canoe</t>
+  </si>
+  <si>
+    <t>cr. controller for canoe</t>
+  </si>
+  <si>
+    <t>cr. class for boat</t>
+  </si>
+  <si>
+    <t>cr. booking view for boat</t>
+  </si>
+  <si>
+    <t>cr. confirmation view for boat</t>
+  </si>
+  <si>
+    <t>cr. controller for boat</t>
+  </si>
+  <si>
+    <t>cr. class for outboard motor</t>
+  </si>
+  <si>
+    <t>cr. booking view for outboard motor</t>
+  </si>
+  <si>
+    <t>cr. confirmation view for outboard motor</t>
+  </si>
+  <si>
+    <t>cr. controller for outboard motor</t>
+  </si>
+  <si>
+    <t>cr. role Recepitonist</t>
+  </si>
+  <si>
+    <t>bughunting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,15 +227,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -201,15 +329,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -507,84 +647,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="12"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="7">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="7" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="7">
+        <v>3</v>
+      </c>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="7">
+        <v>4</v>
+      </c>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="9"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="9"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="4">
-        <v>2</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="4">
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="4">
-        <v>4</v>
-      </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="6"/>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>43262</v>
@@ -647,99 +791,464 @@
         <v>43287</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15.75">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="A29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+    </row>
+    <row r="50" spans="1:22">
+      <c r="A50" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -754,5 +1263,6 @@
     <mergeCell ref="M1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated timeplan for Sprint1
</commit_message>
<xml_diff>
--- a/Camping2000/ProjectFiles/Timeplan.xlsx
+++ b/Camping2000/ProjectFiles/Timeplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deltagare\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FFC78F8-48E7-43A6-9CDA-097B1D52A634}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9A50CE7-9BD3-4BBB-8957-5C3DBDD807AA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>cr = Create</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>cr. database</t>
+  </si>
+  <si>
+    <t>Update all Views with ModelNames</t>
   </si>
   <si>
     <t>cr. registration method</t>
@@ -342,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -368,6 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,11 +652,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V50"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -835,6 +839,7 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" t="s">
@@ -933,6 +938,7 @@
       <c r="B17" t="s">
         <v>5</v>
       </c>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" t="s">
@@ -941,6 +947,7 @@
       <c r="B18" t="s">
         <v>13</v>
       </c>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="4" t="s">
@@ -952,7 +959,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -1043,40 +1050,40 @@
       </c>
     </row>
     <row r="29" spans="1:22">
-      <c r="A29" s="4" t="s">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" t="s">
+      <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
+      <c r="B30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
     </row>
     <row r="31" spans="1:22">
       <c r="A31" t="s">
@@ -1091,15 +1098,15 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1107,7 +1114,7 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1115,7 +1122,7 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1123,7 +1130,7 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1131,7 +1138,7 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1139,7 +1146,7 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1147,7 +1154,7 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1155,7 +1162,7 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1163,7 +1170,7 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1171,7 +1178,7 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1179,7 +1186,7 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1187,7 +1194,7 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1195,7 +1202,7 @@
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1203,7 +1210,7 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1211,7 +1218,7 @@
         <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1219,36 +1226,44 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:22">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-      <c r="V49" s="4"/>
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="50" spans="1:22">
-      <c r="A50" t="s">
-        <v>52</v>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+    </row>
+    <row r="51" spans="1:22">
+      <c r="A51" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check in and checkout is complete. More testing is needed on checkout.
</commit_message>
<xml_diff>
--- a/Camping2000/ProjectFiles/Timeplan.xlsx
+++ b/Camping2000/ProjectFiles/Timeplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deltagare\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA3DEAC1-9489-49A3-B3E2-16303808D85A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95AF2FF7-8E7A-41FF-A5FB-9A907A41C5AE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,8 +627,8 @@
   <dimension ref="A1:V51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q26" sqref="Q26"/>
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1018,6 +1018,7 @@
       <c r="B27" t="s">
         <v>5</v>
       </c>
+      <c r="R27" s="6"/>
     </row>
     <row r="28" spans="1:22">
       <c r="A28" t="s">
@@ -1026,6 +1027,7 @@
       <c r="B28" t="s">
         <v>5</v>
       </c>
+      <c r="R28" s="6"/>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" t="s">

</xml_diff>

<commit_message>
Modify guest data is complete. Work on modify bookingdata is started.
</commit_message>
<xml_diff>
--- a/Camping2000/ProjectFiles/Timeplan.xlsx
+++ b/Camping2000/ProjectFiles/Timeplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20705"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deltagare\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13DDFDB6-9A69-439D-9604-AD33F13C1602}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEC18EF4-5D89-4FDB-8D71-AB9287640DC2}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -313,11 +313,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -344,6 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,11 +636,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V51"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S23" sqref="S23"/>
+      <pane ySplit="3" topLeftCell="R19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W30" sqref="W30:AA30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -636,7 +648,7 @@
     <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +681,7 @@
       <c r="U1" s="12"/>
       <c r="V1" s="13"/>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:27">
       <c r="C2" s="8">
         <v>1</v>
       </c>
@@ -699,7 +711,7 @@
       <c r="U2" s="9"/>
       <c r="V2" s="10"/>
     </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -763,11 +775,26 @@
       <c r="U3" s="2">
         <v>43286</v>
       </c>
-      <c r="V3" s="3">
+      <c r="V3" s="2">
         <v>43287</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="15.75">
+      <c r="W3" s="14">
+        <v>43290</v>
+      </c>
+      <c r="X3" s="2">
+        <v>43291</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>43292</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>43293</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>43294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -795,7 +822,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:27">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -804,7 +831,7 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:27">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -813,7 +840,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:27">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -822,7 +849,7 @@
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:27">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -831,7 +858,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:27">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -840,7 +867,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:27">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -849,7 +876,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:27">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -858,7 +885,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:27">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -867,7 +894,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:27">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -876,7 +903,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:27">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -885,7 +912,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:27">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -894,7 +921,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:27">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -903,7 +930,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:27">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -912,7 +939,7 @@
       </c>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:27">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -921,7 +948,7 @@
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:27">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -949,7 +976,7 @@
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:27">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -958,7 +985,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:27">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -967,7 +994,7 @@
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:27">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -976,7 +1003,7 @@
       </c>
       <c r="O22" s="6"/>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:27">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -985,7 +1012,7 @@
       </c>
       <c r="S23" s="6"/>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:27">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -994,7 +1021,7 @@
       </c>
       <c r="Q24" s="6"/>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:27">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1003,7 +1030,7 @@
       </c>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:27">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1012,7 +1039,7 @@
       </c>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:27">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1021,7 +1048,7 @@
       </c>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:27">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1030,7 +1057,7 @@
       </c>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:27">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1038,7 +1065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:27">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
@@ -1065,8 +1092,13 @@
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
-    </row>
-    <row r="31" spans="1:22">
+      <c r="W30" s="4"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+    </row>
+    <row r="31" spans="1:27">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1074,7 +1106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:27">
       <c r="A32" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
All Core Features are implemented. More bug hunting to do and fail proving. Cleaning of code is neccesary.
</commit_message>
<xml_diff>
--- a/Camping2000/ProjectFiles/Timeplan.xlsx
+++ b/Camping2000/ProjectFiles/Timeplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20705"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deltagare\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEC18EF4-5D89-4FDB-8D71-AB9287640DC2}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4806AA8-8A8E-4CC7-80B3-8ED2C077C77B}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,6 +337,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -355,7 +356,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,8 +639,8 @@
   <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="3" topLeftCell="R19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W30" sqref="W30:AA30"/>
+      <pane ySplit="3" topLeftCell="D21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -652,64 +652,64 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="11" t="s">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="11" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="11" t="s">
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="14"/>
     </row>
     <row r="2" spans="1:27">
-      <c r="C2" s="8">
+      <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="8">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="9">
         <v>2</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="8">
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="9">
         <v>3</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="8">
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="9">
         <v>4</v>
       </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="11"/>
     </row>
     <row r="3" spans="1:27">
       <c r="A3" t="s">
@@ -778,7 +778,7 @@
       <c r="V3" s="2">
         <v>43287</v>
       </c>
-      <c r="W3" s="14">
+      <c r="W3" s="8">
         <v>43290</v>
       </c>
       <c r="X3" s="2">
@@ -1064,6 +1064,7 @@
       <c r="B29" t="s">
         <v>5</v>
       </c>
+      <c r="AA29" s="6"/>
     </row>
     <row r="30" spans="1:27">
       <c r="A30" s="4" t="s">

</xml_diff>

<commit_message>
Work on listing all current receptionists have started but is not complete
</commit_message>
<xml_diff>
--- a/Camping2000/ProjectFiles/Timeplan.xlsx
+++ b/Camping2000/ProjectFiles/Timeplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deltagare\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75EC8BCB-3565-4341-A670-3DAF872AC4B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A45C9D5-4DE3-4560-983D-5A12F12497E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,17 +357,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -380,25 +394,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -684,8 +679,8 @@
   <dimension ref="A1:AK51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane xSplit="2" ySplit="3" topLeftCell="V34" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AG51" sqref="AG51:AH51"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="X39" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AI49" sqref="AI49"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -699,106 +694,106 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="9" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="9" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="9" t="s">
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="6" t="s">
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="24" t="s">
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="24" t="s">
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="7"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
     </row>
     <row r="2" spans="1:37">
-      <c r="C2" s="6">
+      <c r="C2" s="16">
         <v>1</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="6">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="16">
         <v>2</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="6">
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="16">
         <v>3</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="6">
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="16">
         <v>4</v>
       </c>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="6">
-        <v>5</v>
-      </c>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="24">
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="16">
+        <v>5</v>
+      </c>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="14">
         <v>6</v>
       </c>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="24">
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="14">
         <v>7</v>
       </c>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
+      <c r="AH2" s="15"/>
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
     </row>
     <row r="3" spans="1:37">
       <c r="A3" t="s">
@@ -864,7 +859,7 @@
       <c r="U3" s="2">
         <v>43286</v>
       </c>
-      <c r="V3" s="20">
+      <c r="V3" s="12">
         <v>43287</v>
       </c>
       <c r="W3" s="2">
@@ -879,7 +874,7 @@
       <c r="Z3" s="2">
         <v>43293</v>
       </c>
-      <c r="AA3" s="20">
+      <c r="AA3" s="12">
         <v>43294</v>
       </c>
       <c r="AB3" s="4">
@@ -894,7 +889,7 @@
       <c r="AE3" s="4">
         <v>43314</v>
       </c>
-      <c r="AF3" s="16">
+      <c r="AF3" s="8">
         <v>43315</v>
       </c>
       <c r="AG3" s="4">
@@ -924,28 +919,24 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="16"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="16"/>
+      <c r="L4" s="8"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="16"/>
+      <c r="Q4" s="8"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="17"/>
-      <c r="AF4" s="17"/>
+      <c r="V4" s="8"/>
+      <c r="AA4" s="9"/>
+      <c r="AF4" s="9"/>
     </row>
     <row r="5" spans="1:37">
       <c r="A5" t="s">
@@ -955,16 +946,12 @@
         <v>5</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="G5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="17"/>
-      <c r="AF5" s="17"/>
+      <c r="G5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AF5" s="9"/>
     </row>
     <row r="6" spans="1:37">
       <c r="A6" t="s">
@@ -974,16 +961,12 @@
         <v>5</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="17"/>
-      <c r="AF6" s="17"/>
+      <c r="G6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AF6" s="9"/>
     </row>
     <row r="7" spans="1:37">
       <c r="A7" t="s">
@@ -993,16 +976,12 @@
         <v>5</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="G7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="17"/>
-      <c r="AF7" s="17"/>
+      <c r="G7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AF7" s="9"/>
     </row>
     <row r="8" spans="1:37">
       <c r="A8" t="s">
@@ -1012,16 +991,12 @@
         <v>5</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="G8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="17"/>
-      <c r="AF8" s="17"/>
+      <c r="G8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AF8" s="9"/>
     </row>
     <row r="9" spans="1:37">
       <c r="A9" t="s">
@@ -1031,16 +1006,12 @@
         <v>5</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="G9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="17"/>
-      <c r="AF9" s="17"/>
+      <c r="G9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AF9" s="9"/>
     </row>
     <row r="10" spans="1:37">
       <c r="A10" t="s">
@@ -1050,16 +1021,12 @@
         <v>5</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="G10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="17"/>
-      <c r="AF10" s="17"/>
+      <c r="G10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AF10" s="9"/>
     </row>
     <row r="11" spans="1:37">
       <c r="A11" t="s">
@@ -1069,16 +1036,12 @@
         <v>13</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="G11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="17"/>
-      <c r="AF11" s="17"/>
+      <c r="G11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AF11" s="9"/>
     </row>
     <row r="12" spans="1:37">
       <c r="A12" t="s">
@@ -1088,16 +1051,12 @@
         <v>5</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="G12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="V12" s="17"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="17"/>
-      <c r="AF12" s="17"/>
+      <c r="G12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AF12" s="9"/>
     </row>
     <row r="13" spans="1:37">
       <c r="A13" t="s">
@@ -1107,16 +1066,12 @@
         <v>13</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="G13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="V13" s="17"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="17"/>
-      <c r="AF13" s="17"/>
+      <c r="G13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AF13" s="9"/>
     </row>
     <row r="14" spans="1:37">
       <c r="A14" t="s">
@@ -1126,16 +1081,12 @@
         <v>5</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="G14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="17"/>
-      <c r="AF14" s="17"/>
+      <c r="G14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AF14" s="9"/>
     </row>
     <row r="15" spans="1:37">
       <c r="A15" t="s">
@@ -1145,16 +1096,12 @@
         <v>5</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="G15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="V15" s="17"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
-      <c r="Y15" s="13"/>
-      <c r="Z15" s="13"/>
-      <c r="AA15" s="17"/>
-      <c r="AF15" s="17"/>
+      <c r="G15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AF15" s="9"/>
     </row>
     <row r="16" spans="1:37">
       <c r="A16" t="s">
@@ -1164,16 +1111,12 @@
         <v>13</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="G16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="V16" s="17"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="13"/>
-      <c r="Z16" s="13"/>
-      <c r="AA16" s="17"/>
-      <c r="AF16" s="17"/>
+      <c r="G16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AF16" s="9"/>
     </row>
     <row r="17" spans="1:32">
       <c r="A17" t="s">
@@ -1183,16 +1126,12 @@
         <v>5</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="G17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="V17" s="17"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="17"/>
-      <c r="AF17" s="17"/>
+      <c r="G17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AF17" s="9"/>
     </row>
     <row r="18" spans="1:32">
       <c r="A18" t="s">
@@ -1202,65 +1141,42 @@
         <v>13</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="G18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="V18" s="17"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
-      <c r="AA18" s="17"/>
-      <c r="AF18" s="17"/>
+      <c r="G18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AF18" s="9"/>
     </row>
     <row r="19" spans="1:32">
-      <c r="A19" s="13" t="s">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="17"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
-      <c r="AA19" s="17"/>
-      <c r="AF19" s="17"/>
-    </row>
-    <row r="20" spans="1:32" s="12" customFormat="1">
-      <c r="A20" s="12" t="s">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AF19" s="9"/>
+    </row>
+    <row r="20" spans="1:32" s="6" customFormat="1">
+      <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="18"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="AA20" s="18"/>
-      <c r="AF20" s="18"/>
+      <c r="B20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AF20" s="10"/>
     </row>
     <row r="21" spans="1:32">
       <c r="A21" t="s">
@@ -1269,17 +1185,13 @@
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="17"/>
+      <c r="G21" s="9"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="V21" s="17"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
-      <c r="Z21" s="13"/>
-      <c r="AA21" s="17"/>
-      <c r="AF21" s="17"/>
+      <c r="L21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AF21" s="9"/>
     </row>
     <row r="22" spans="1:32">
       <c r="A22" t="s">
@@ -1288,17 +1200,13 @@
       <c r="B22" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="L22" s="17"/>
+      <c r="G22" s="9"/>
+      <c r="L22" s="9"/>
       <c r="O22" s="5"/>
-      <c r="Q22" s="17"/>
-      <c r="V22" s="17"/>
-      <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
-      <c r="AA22" s="17"/>
-      <c r="AF22" s="17"/>
+      <c r="Q22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AF22" s="9"/>
     </row>
     <row r="23" spans="1:32">
       <c r="A23" t="s">
@@ -1307,17 +1215,13 @@
       <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="Q23" s="17"/>
+      <c r="G23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="Q23" s="9"/>
       <c r="S23" s="5"/>
-      <c r="V23" s="17"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="13"/>
-      <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
-      <c r="AA23" s="17"/>
-      <c r="AF23" s="17"/>
+      <c r="V23" s="9"/>
+      <c r="AA23" s="9"/>
+      <c r="AF23" s="9"/>
     </row>
     <row r="24" spans="1:32">
       <c r="A24" t="s">
@@ -1326,16 +1230,12 @@
       <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="Q24" s="19"/>
-      <c r="V24" s="17"/>
-      <c r="W24" s="13"/>
-      <c r="X24" s="13"/>
-      <c r="Y24" s="13"/>
-      <c r="Z24" s="13"/>
-      <c r="AA24" s="17"/>
-      <c r="AF24" s="17"/>
+      <c r="G24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="Q24" s="11"/>
+      <c r="V24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AF24" s="9"/>
     </row>
     <row r="25" spans="1:32">
       <c r="A25" t="s">
@@ -1344,16 +1244,12 @@
       <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="Q25" s="19"/>
-      <c r="V25" s="17"/>
-      <c r="W25" s="13"/>
-      <c r="X25" s="13"/>
-      <c r="Y25" s="13"/>
-      <c r="Z25" s="13"/>
-      <c r="AA25" s="17"/>
-      <c r="AF25" s="17"/>
+      <c r="G25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="Q25" s="11"/>
+      <c r="V25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AF25" s="9"/>
     </row>
     <row r="26" spans="1:32">
       <c r="A26" t="s">
@@ -1362,16 +1258,12 @@
       <c r="B26" t="s">
         <v>5</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="Q26" s="19"/>
-      <c r="V26" s="17"/>
-      <c r="W26" s="13"/>
-      <c r="X26" s="13"/>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="13"/>
-      <c r="AA26" s="17"/>
-      <c r="AF26" s="17"/>
+      <c r="G26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="Q26" s="11"/>
+      <c r="V26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AF26" s="9"/>
     </row>
     <row r="27" spans="1:32">
       <c r="A27" t="s">
@@ -1380,17 +1272,13 @@
       <c r="B27" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="Q27" s="17"/>
+      <c r="G27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="Q27" s="9"/>
       <c r="R27" s="5"/>
-      <c r="V27" s="17"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
-      <c r="AA27" s="17"/>
-      <c r="AF27" s="17"/>
+      <c r="V27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AF27" s="9"/>
     </row>
     <row r="28" spans="1:32">
       <c r="A28" t="s">
@@ -1399,17 +1287,13 @@
       <c r="B28" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="Q28" s="17"/>
+      <c r="G28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="Q28" s="9"/>
       <c r="R28" s="5"/>
-      <c r="V28" s="17"/>
-      <c r="W28" s="13"/>
-      <c r="X28" s="13"/>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="13"/>
-      <c r="AA28" s="17"/>
-      <c r="AF28" s="17"/>
+      <c r="V28" s="9"/>
+      <c r="AA28" s="9"/>
+      <c r="AF28" s="9"/>
     </row>
     <row r="29" spans="1:32">
       <c r="A29" t="s">
@@ -1418,64 +1302,41 @@
       <c r="B29" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="Q29" s="17"/>
-      <c r="V29" s="17"/>
-      <c r="W29" s="13"/>
-      <c r="X29" s="13"/>
-      <c r="Y29" s="13"/>
-      <c r="Z29" s="13"/>
-      <c r="AA29" s="19"/>
-      <c r="AF29" s="17"/>
+      <c r="G29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="AA29" s="11"/>
+      <c r="AF29" s="9"/>
     </row>
     <row r="30" spans="1:32">
-      <c r="A30" s="13" t="s">
+      <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
-      <c r="U30" s="13"/>
-      <c r="V30" s="17"/>
-      <c r="W30" s="13"/>
-      <c r="X30" s="14"/>
-      <c r="Y30" s="13"/>
-      <c r="Z30" s="13"/>
-      <c r="AA30" s="17"/>
-      <c r="AF30" s="17"/>
-    </row>
-    <row r="31" spans="1:32" s="12" customFormat="1">
-      <c r="A31" s="12" t="s">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="X30" s="5"/>
+      <c r="AA30" s="9"/>
+      <c r="AF30" s="9"/>
+    </row>
+    <row r="31" spans="1:32" s="6" customFormat="1">
+      <c r="A31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="V31" s="18"/>
-      <c r="AA31" s="18"/>
-      <c r="AF31" s="18"/>
+      <c r="G31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="AA31" s="10"/>
+      <c r="AF31" s="10"/>
     </row>
     <row r="32" spans="1:32">
       <c r="A32" t="s">
@@ -1484,16 +1345,12 @@
       <c r="B32" t="s">
         <v>13</v>
       </c>
-      <c r="G32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="V32" s="17"/>
-      <c r="W32" s="13"/>
-      <c r="X32" s="13"/>
-      <c r="Y32" s="13"/>
-      <c r="Z32" s="13"/>
-      <c r="AA32" s="17"/>
-      <c r="AF32" s="17"/>
+      <c r="G32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="AA32" s="9"/>
+      <c r="AF32" s="9"/>
     </row>
     <row r="33" spans="1:32">
       <c r="A33" t="s">
@@ -1502,16 +1359,12 @@
       <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="Q33" s="17"/>
-      <c r="V33" s="17"/>
-      <c r="W33" s="13"/>
-      <c r="X33" s="13"/>
-      <c r="Y33" s="13"/>
-      <c r="Z33" s="13"/>
-      <c r="AA33" s="17"/>
-      <c r="AF33" s="17"/>
+      <c r="G33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="AA33" s="9"/>
+      <c r="AF33" s="9"/>
     </row>
     <row r="34" spans="1:32">
       <c r="A34" t="s">
@@ -1520,16 +1373,12 @@
       <c r="B34" t="s">
         <v>36</v>
       </c>
-      <c r="G34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="Q34" s="17"/>
-      <c r="V34" s="17"/>
-      <c r="W34" s="13"/>
-      <c r="X34" s="13"/>
-      <c r="Y34" s="13"/>
-      <c r="Z34" s="13"/>
-      <c r="AA34" s="17"/>
-      <c r="AF34" s="17"/>
+      <c r="G34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="V34" s="9"/>
+      <c r="AA34" s="9"/>
+      <c r="AF34" s="9"/>
     </row>
     <row r="35" spans="1:32">
       <c r="A35" t="s">
@@ -1538,16 +1387,12 @@
       <c r="B35" t="s">
         <v>36</v>
       </c>
-      <c r="G35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="V35" s="17"/>
-      <c r="W35" s="13"/>
-      <c r="X35" s="13"/>
-      <c r="Y35" s="13"/>
-      <c r="Z35" s="13"/>
-      <c r="AA35" s="17"/>
-      <c r="AF35" s="17"/>
+      <c r="G35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="V35" s="9"/>
+      <c r="AA35" s="9"/>
+      <c r="AF35" s="9"/>
     </row>
     <row r="36" spans="1:32">
       <c r="A36" t="s">
@@ -1556,16 +1401,12 @@
       <c r="B36" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="Q36" s="17"/>
-      <c r="V36" s="17"/>
-      <c r="W36" s="13"/>
-      <c r="X36" s="13"/>
-      <c r="Y36" s="13"/>
-      <c r="Z36" s="13"/>
-      <c r="AA36" s="17"/>
-      <c r="AF36" s="17"/>
+      <c r="G36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="V36" s="9"/>
+      <c r="AA36" s="9"/>
+      <c r="AF36" s="9"/>
     </row>
     <row r="37" spans="1:32">
       <c r="A37" t="s">
@@ -1574,16 +1415,12 @@
       <c r="B37" t="s">
         <v>36</v>
       </c>
-      <c r="G37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="Q37" s="17"/>
-      <c r="V37" s="17"/>
-      <c r="W37" s="13"/>
-      <c r="X37" s="13"/>
-      <c r="Y37" s="13"/>
-      <c r="Z37" s="13"/>
-      <c r="AA37" s="17"/>
-      <c r="AF37" s="17"/>
+      <c r="G37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="V37" s="9"/>
+      <c r="AA37" s="9"/>
+      <c r="AF37" s="9"/>
     </row>
     <row r="38" spans="1:32">
       <c r="A38" t="s">
@@ -1592,16 +1429,12 @@
       <c r="B38" t="s">
         <v>36</v>
       </c>
-      <c r="G38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="Q38" s="17"/>
-      <c r="V38" s="17"/>
-      <c r="W38" s="13"/>
-      <c r="X38" s="13"/>
-      <c r="Y38" s="13"/>
-      <c r="Z38" s="13"/>
-      <c r="AA38" s="17"/>
-      <c r="AF38" s="17"/>
+      <c r="G38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="V38" s="9"/>
+      <c r="AA38" s="9"/>
+      <c r="AF38" s="9"/>
     </row>
     <row r="39" spans="1:32">
       <c r="A39" t="s">
@@ -1610,16 +1443,12 @@
       <c r="B39" t="s">
         <v>36</v>
       </c>
-      <c r="G39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="Q39" s="17"/>
-      <c r="V39" s="17"/>
-      <c r="W39" s="13"/>
-      <c r="X39" s="13"/>
-      <c r="Y39" s="13"/>
-      <c r="Z39" s="13"/>
-      <c r="AA39" s="17"/>
-      <c r="AF39" s="17"/>
+      <c r="G39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="V39" s="9"/>
+      <c r="AA39" s="9"/>
+      <c r="AF39" s="9"/>
     </row>
     <row r="40" spans="1:32">
       <c r="A40" t="s">
@@ -1628,16 +1457,12 @@
       <c r="B40" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="Q40" s="17"/>
-      <c r="V40" s="17"/>
-      <c r="W40" s="13"/>
-      <c r="X40" s="13"/>
-      <c r="Y40" s="13"/>
-      <c r="Z40" s="13"/>
-      <c r="AA40" s="17"/>
-      <c r="AF40" s="17"/>
+      <c r="G40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="V40" s="9"/>
+      <c r="AA40" s="9"/>
+      <c r="AF40" s="9"/>
     </row>
     <row r="41" spans="1:32">
       <c r="A41" t="s">
@@ -1646,16 +1471,12 @@
       <c r="B41" t="s">
         <v>36</v>
       </c>
-      <c r="G41" s="17"/>
-      <c r="L41" s="17"/>
-      <c r="Q41" s="17"/>
-      <c r="V41" s="17"/>
-      <c r="W41" s="13"/>
-      <c r="X41" s="13"/>
-      <c r="Y41" s="13"/>
-      <c r="Z41" s="13"/>
-      <c r="AA41" s="17"/>
-      <c r="AF41" s="17"/>
+      <c r="G41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="V41" s="9"/>
+      <c r="AA41" s="9"/>
+      <c r="AF41" s="9"/>
     </row>
     <row r="42" spans="1:32">
       <c r="A42" t="s">
@@ -1664,16 +1485,12 @@
       <c r="B42" t="s">
         <v>36</v>
       </c>
-      <c r="G42" s="17"/>
-      <c r="L42" s="17"/>
-      <c r="Q42" s="17"/>
-      <c r="V42" s="17"/>
-      <c r="W42" s="13"/>
-      <c r="X42" s="13"/>
-      <c r="Y42" s="13"/>
-      <c r="Z42" s="13"/>
-      <c r="AA42" s="17"/>
-      <c r="AF42" s="17"/>
+      <c r="G42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="V42" s="9"/>
+      <c r="AA42" s="9"/>
+      <c r="AF42" s="9"/>
     </row>
     <row r="43" spans="1:32">
       <c r="A43" t="s">
@@ -1682,16 +1499,12 @@
       <c r="B43" t="s">
         <v>36</v>
       </c>
-      <c r="G43" s="17"/>
-      <c r="L43" s="17"/>
-      <c r="Q43" s="17"/>
-      <c r="V43" s="17"/>
-      <c r="W43" s="13"/>
-      <c r="X43" s="13"/>
-      <c r="Y43" s="13"/>
-      <c r="Z43" s="13"/>
-      <c r="AA43" s="17"/>
-      <c r="AF43" s="17"/>
+      <c r="G43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="V43" s="9"/>
+      <c r="AA43" s="9"/>
+      <c r="AF43" s="9"/>
     </row>
     <row r="44" spans="1:32">
       <c r="A44" t="s">
@@ -1700,16 +1513,12 @@
       <c r="B44" t="s">
         <v>36</v>
       </c>
-      <c r="G44" s="17"/>
-      <c r="L44" s="17"/>
-      <c r="Q44" s="17"/>
-      <c r="V44" s="17"/>
-      <c r="W44" s="13"/>
-      <c r="X44" s="13"/>
-      <c r="Y44" s="13"/>
-      <c r="Z44" s="13"/>
-      <c r="AA44" s="17"/>
-      <c r="AF44" s="17"/>
+      <c r="G44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="Q44" s="9"/>
+      <c r="V44" s="9"/>
+      <c r="AA44" s="9"/>
+      <c r="AF44" s="9"/>
     </row>
     <row r="45" spans="1:32">
       <c r="A45" t="s">
@@ -1718,16 +1527,12 @@
       <c r="B45" t="s">
         <v>36</v>
       </c>
-      <c r="G45" s="17"/>
-      <c r="L45" s="17"/>
-      <c r="Q45" s="17"/>
-      <c r="V45" s="17"/>
-      <c r="W45" s="13"/>
-      <c r="X45" s="13"/>
-      <c r="Y45" s="13"/>
-      <c r="Z45" s="13"/>
-      <c r="AA45" s="17"/>
-      <c r="AF45" s="17"/>
+      <c r="G45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="Q45" s="9"/>
+      <c r="V45" s="9"/>
+      <c r="AA45" s="9"/>
+      <c r="AF45" s="9"/>
     </row>
     <row r="46" spans="1:32">
       <c r="A46" t="s">
@@ -1736,16 +1541,12 @@
       <c r="B46" t="s">
         <v>36</v>
       </c>
-      <c r="G46" s="17"/>
-      <c r="L46" s="17"/>
-      <c r="Q46" s="17"/>
-      <c r="V46" s="17"/>
-      <c r="W46" s="13"/>
-      <c r="X46" s="13"/>
-      <c r="Y46" s="13"/>
-      <c r="Z46" s="13"/>
-      <c r="AA46" s="17"/>
-      <c r="AF46" s="17"/>
+      <c r="G46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="Q46" s="9"/>
+      <c r="V46" s="9"/>
+      <c r="AA46" s="9"/>
+      <c r="AF46" s="9"/>
     </row>
     <row r="47" spans="1:32">
       <c r="A47" t="s">
@@ -1754,16 +1555,12 @@
       <c r="B47" t="s">
         <v>36</v>
       </c>
-      <c r="G47" s="17"/>
-      <c r="L47" s="17"/>
-      <c r="Q47" s="17"/>
-      <c r="V47" s="17"/>
-      <c r="W47" s="13"/>
-      <c r="X47" s="13"/>
-      <c r="Y47" s="13"/>
-      <c r="Z47" s="13"/>
-      <c r="AA47" s="17"/>
-      <c r="AF47" s="17"/>
+      <c r="G47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="Q47" s="9"/>
+      <c r="V47" s="9"/>
+      <c r="AA47" s="9"/>
+      <c r="AF47" s="9"/>
     </row>
     <row r="48" spans="1:32">
       <c r="A48" t="s">
@@ -1772,90 +1569,55 @@
       <c r="B48" t="s">
         <v>36</v>
       </c>
-      <c r="G48" s="17"/>
-      <c r="L48" s="17"/>
-      <c r="Q48" s="17"/>
-      <c r="V48" s="17"/>
-      <c r="W48" s="13"/>
-      <c r="X48" s="13"/>
-      <c r="Y48" s="13"/>
-      <c r="Z48" s="13"/>
-      <c r="AA48" s="17"/>
-      <c r="AF48" s="17"/>
-    </row>
-    <row r="49" spans="1:34">
+      <c r="G48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="Q48" s="9"/>
+      <c r="V48" s="9"/>
+      <c r="AA48" s="9"/>
+      <c r="AF48" s="9"/>
+    </row>
+    <row r="49" spans="1:35">
       <c r="A49" t="s">
         <v>52</v>
       </c>
       <c r="B49" t="s">
         <v>36</v>
       </c>
-      <c r="G49" s="17"/>
-      <c r="L49" s="17"/>
-      <c r="Q49" s="17"/>
-      <c r="V49" s="17"/>
-      <c r="W49" s="13"/>
-      <c r="X49" s="13"/>
-      <c r="Y49" s="13"/>
-      <c r="Z49" s="13"/>
-      <c r="AA49" s="17"/>
-      <c r="AF49" s="17"/>
-    </row>
-    <row r="50" spans="1:34">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="17"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="13"/>
-      <c r="Q50" s="17"/>
-      <c r="R50" s="13"/>
-      <c r="S50" s="13"/>
-      <c r="T50" s="13"/>
-      <c r="U50" s="13"/>
-      <c r="V50" s="17"/>
-      <c r="W50" s="13"/>
-      <c r="X50" s="13"/>
-      <c r="Y50" s="13"/>
-      <c r="Z50" s="13"/>
-      <c r="AA50" s="17"/>
-      <c r="AF50" s="17"/>
-    </row>
-    <row r="51" spans="1:34" s="12" customFormat="1">
-      <c r="A51" s="12" t="s">
+      <c r="G49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="Q49" s="9"/>
+      <c r="V49" s="9"/>
+      <c r="AA49" s="9"/>
+      <c r="AF49" s="9"/>
+      <c r="AI49" s="5"/>
+    </row>
+    <row r="50" spans="1:35">
+      <c r="G50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="V50" s="9"/>
+      <c r="AA50" s="9"/>
+      <c r="AF50" s="9"/>
+    </row>
+    <row r="51" spans="1:35" s="6" customFormat="1">
+      <c r="A51" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="Q51" s="18"/>
-      <c r="V51" s="18"/>
-      <c r="AA51" s="18"/>
-      <c r="AB51" s="15"/>
-      <c r="AC51" s="15"/>
-      <c r="AD51" s="15"/>
-      <c r="AE51" s="15"/>
-      <c r="AF51" s="23"/>
-      <c r="AG51" s="15"/>
-      <c r="AH51" s="15"/>
+      <c r="G51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="V51" s="10"/>
+      <c r="AA51" s="10"/>
+      <c r="AB51" s="7"/>
+      <c r="AC51" s="7"/>
+      <c r="AD51" s="7"/>
+      <c r="AE51" s="7"/>
+      <c r="AF51" s="13"/>
+      <c r="AG51" s="7"/>
+      <c r="AH51" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="AG1:AK1"/>
-    <mergeCell ref="AG2:AK2"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="W2:AA2"/>
-    <mergeCell ref="AB1:AF1"/>
-    <mergeCell ref="AB2:AF2"/>
     <mergeCell ref="R2:V2"/>
     <mergeCell ref="R1:V1"/>
     <mergeCell ref="C2:G2"/>
@@ -1864,6 +1626,12 @@
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="AG1:AK1"/>
+    <mergeCell ref="AG2:AK2"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="AB2:AF2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
work on continue a reservation after login or registration have begun.
</commit_message>
<xml_diff>
--- a/Camping2000/ProjectFiles/Timeplan.xlsx
+++ b/Camping2000/ProjectFiles/Timeplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20823"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deltagare\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A45C9D5-4DE3-4560-983D-5A12F12497E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5102850-C9B8-4A3C-915F-4766BDE86D38}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t>cr = Create</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>cr. role Recepitonist</t>
+  </si>
+  <si>
+    <t>Validate fetched data</t>
   </si>
   <si>
     <t>bughunting</t>
@@ -216,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -353,11 +356,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -396,6 +410,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,11 +693,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK51"/>
+  <dimension ref="A1:AP51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane xSplit="2" ySplit="3" topLeftCell="X39" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AI49" sqref="AI49"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AD44" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AL51" sqref="AL51"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -690,7 +707,7 @@
     <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:42">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -743,8 +760,9 @@
       <c r="AI1" s="15"/>
       <c r="AJ1" s="15"/>
       <c r="AK1" s="15"/>
-    </row>
-    <row r="2" spans="1:37">
+      <c r="AL1" s="22"/>
+    </row>
+    <row r="2" spans="1:42">
       <c r="C2" s="16">
         <v>1</v>
       </c>
@@ -794,8 +812,9 @@
       <c r="AI2" s="15"/>
       <c r="AJ2" s="15"/>
       <c r="AK2" s="15"/>
-    </row>
-    <row r="3" spans="1:37">
+      <c r="AL2" s="22"/>
+    </row>
+    <row r="3" spans="1:42">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -907,8 +926,23 @@
       <c r="AK3" s="4">
         <v>43329</v>
       </c>
-    </row>
-    <row r="4" spans="1:37">
+      <c r="AL3" s="24">
+        <v>43332</v>
+      </c>
+      <c r="AM3" s="4">
+        <v>43333</v>
+      </c>
+      <c r="AN3" s="4">
+        <v>43334</v>
+      </c>
+      <c r="AO3" s="4">
+        <v>43335</v>
+      </c>
+      <c r="AP3" s="4">
+        <v>43336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -937,8 +971,9 @@
       <c r="V4" s="8"/>
       <c r="AA4" s="9"/>
       <c r="AF4" s="9"/>
-    </row>
-    <row r="5" spans="1:37">
+      <c r="AL4" s="22"/>
+    </row>
+    <row r="5" spans="1:42">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -952,8 +987,9 @@
       <c r="V5" s="9"/>
       <c r="AA5" s="9"/>
       <c r="AF5" s="9"/>
-    </row>
-    <row r="6" spans="1:37">
+      <c r="AL5" s="22"/>
+    </row>
+    <row r="6" spans="1:42">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -967,8 +1003,9 @@
       <c r="V6" s="9"/>
       <c r="AA6" s="9"/>
       <c r="AF6" s="9"/>
-    </row>
-    <row r="7" spans="1:37">
+      <c r="AL6" s="22"/>
+    </row>
+    <row r="7" spans="1:42">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -982,8 +1019,9 @@
       <c r="V7" s="9"/>
       <c r="AA7" s="9"/>
       <c r="AF7" s="9"/>
-    </row>
-    <row r="8" spans="1:37">
+      <c r="AL7" s="22"/>
+    </row>
+    <row r="8" spans="1:42">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -997,8 +1035,9 @@
       <c r="V8" s="9"/>
       <c r="AA8" s="9"/>
       <c r="AF8" s="9"/>
-    </row>
-    <row r="9" spans="1:37">
+      <c r="AL8" s="22"/>
+    </row>
+    <row r="9" spans="1:42">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1012,8 +1051,9 @@
       <c r="V9" s="9"/>
       <c r="AA9" s="9"/>
       <c r="AF9" s="9"/>
-    </row>
-    <row r="10" spans="1:37">
+      <c r="AL9" s="22"/>
+    </row>
+    <row r="10" spans="1:42">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1027,8 +1067,9 @@
       <c r="V10" s="9"/>
       <c r="AA10" s="9"/>
       <c r="AF10" s="9"/>
-    </row>
-    <row r="11" spans="1:37">
+      <c r="AL10" s="22"/>
+    </row>
+    <row r="11" spans="1:42">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1042,8 +1083,9 @@
       <c r="V11" s="9"/>
       <c r="AA11" s="9"/>
       <c r="AF11" s="9"/>
-    </row>
-    <row r="12" spans="1:37">
+      <c r="AL11" s="22"/>
+    </row>
+    <row r="12" spans="1:42">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1057,8 +1099,9 @@
       <c r="V12" s="9"/>
       <c r="AA12" s="9"/>
       <c r="AF12" s="9"/>
-    </row>
-    <row r="13" spans="1:37">
+      <c r="AL12" s="22"/>
+    </row>
+    <row r="13" spans="1:42">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1072,8 +1115,9 @@
       <c r="V13" s="9"/>
       <c r="AA13" s="9"/>
       <c r="AF13" s="9"/>
-    </row>
-    <row r="14" spans="1:37">
+      <c r="AL13" s="22"/>
+    </row>
+    <row r="14" spans="1:42">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1087,8 +1131,9 @@
       <c r="V14" s="9"/>
       <c r="AA14" s="9"/>
       <c r="AF14" s="9"/>
-    </row>
-    <row r="15" spans="1:37">
+      <c r="AL14" s="22"/>
+    </row>
+    <row r="15" spans="1:42">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1102,8 +1147,9 @@
       <c r="V15" s="9"/>
       <c r="AA15" s="9"/>
       <c r="AF15" s="9"/>
-    </row>
-    <row r="16" spans="1:37">
+      <c r="AL15" s="22"/>
+    </row>
+    <row r="16" spans="1:42">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1117,8 +1163,9 @@
       <c r="V16" s="9"/>
       <c r="AA16" s="9"/>
       <c r="AF16" s="9"/>
-    </row>
-    <row r="17" spans="1:32">
+      <c r="AL16" s="22"/>
+    </row>
+    <row r="17" spans="1:38">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1132,8 +1179,9 @@
       <c r="V17" s="9"/>
       <c r="AA17" s="9"/>
       <c r="AF17" s="9"/>
-    </row>
-    <row r="18" spans="1:32">
+      <c r="AL17" s="22"/>
+    </row>
+    <row r="18" spans="1:38">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1147,8 +1195,9 @@
       <c r="V18" s="9"/>
       <c r="AA18" s="9"/>
       <c r="AF18" s="9"/>
-    </row>
-    <row r="19" spans="1:32">
+      <c r="AL18" s="22"/>
+    </row>
+    <row r="19" spans="1:38">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1162,8 +1211,9 @@
       <c r="V19" s="9"/>
       <c r="AA19" s="9"/>
       <c r="AF19" s="9"/>
-    </row>
-    <row r="20" spans="1:32" s="6" customFormat="1">
+      <c r="AL19" s="22"/>
+    </row>
+    <row r="20" spans="1:38" s="6" customFormat="1">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
@@ -1177,8 +1227,9 @@
       <c r="V20" s="10"/>
       <c r="AA20" s="10"/>
       <c r="AF20" s="10"/>
-    </row>
-    <row r="21" spans="1:32">
+      <c r="AL20" s="23"/>
+    </row>
+    <row r="21" spans="1:38">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1192,8 +1243,9 @@
       <c r="V21" s="9"/>
       <c r="AA21" s="9"/>
       <c r="AF21" s="9"/>
-    </row>
-    <row r="22" spans="1:32">
+      <c r="AL21" s="22"/>
+    </row>
+    <row r="22" spans="1:38">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1207,8 +1259,9 @@
       <c r="V22" s="9"/>
       <c r="AA22" s="9"/>
       <c r="AF22" s="9"/>
-    </row>
-    <row r="23" spans="1:32">
+      <c r="AL22" s="22"/>
+    </row>
+    <row r="23" spans="1:38">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1222,8 +1275,9 @@
       <c r="V23" s="9"/>
       <c r="AA23" s="9"/>
       <c r="AF23" s="9"/>
-    </row>
-    <row r="24" spans="1:32">
+      <c r="AL23" s="22"/>
+    </row>
+    <row r="24" spans="1:38">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1236,8 +1290,9 @@
       <c r="V24" s="9"/>
       <c r="AA24" s="9"/>
       <c r="AF24" s="9"/>
-    </row>
-    <row r="25" spans="1:32">
+      <c r="AL24" s="22"/>
+    </row>
+    <row r="25" spans="1:38">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1250,8 +1305,9 @@
       <c r="V25" s="9"/>
       <c r="AA25" s="9"/>
       <c r="AF25" s="9"/>
-    </row>
-    <row r="26" spans="1:32">
+      <c r="AL25" s="22"/>
+    </row>
+    <row r="26" spans="1:38">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1264,8 +1320,9 @@
       <c r="V26" s="9"/>
       <c r="AA26" s="9"/>
       <c r="AF26" s="9"/>
-    </row>
-    <row r="27" spans="1:32">
+      <c r="AL26" s="22"/>
+    </row>
+    <row r="27" spans="1:38">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1279,8 +1336,9 @@
       <c r="V27" s="9"/>
       <c r="AA27" s="9"/>
       <c r="AF27" s="9"/>
-    </row>
-    <row r="28" spans="1:32">
+      <c r="AL27" s="22"/>
+    </row>
+    <row r="28" spans="1:38">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1294,8 +1352,9 @@
       <c r="V28" s="9"/>
       <c r="AA28" s="9"/>
       <c r="AF28" s="9"/>
-    </row>
-    <row r="29" spans="1:32">
+      <c r="AL28" s="22"/>
+    </row>
+    <row r="29" spans="1:38">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1308,8 +1367,9 @@
       <c r="V29" s="9"/>
       <c r="AA29" s="11"/>
       <c r="AF29" s="9"/>
-    </row>
-    <row r="30" spans="1:32">
+      <c r="AL29" s="22"/>
+    </row>
+    <row r="30" spans="1:38">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1323,8 +1383,9 @@
       <c r="X30" s="5"/>
       <c r="AA30" s="9"/>
       <c r="AF30" s="9"/>
-    </row>
-    <row r="31" spans="1:32" s="6" customFormat="1">
+      <c r="AL30" s="22"/>
+    </row>
+    <row r="31" spans="1:38" s="6" customFormat="1">
       <c r="A31" s="6" t="s">
         <v>33</v>
       </c>
@@ -1337,8 +1398,9 @@
       <c r="V31" s="10"/>
       <c r="AA31" s="10"/>
       <c r="AF31" s="10"/>
-    </row>
-    <row r="32" spans="1:32">
+      <c r="AL31" s="23"/>
+    </row>
+    <row r="32" spans="1:38">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1351,8 +1413,9 @@
       <c r="V32" s="9"/>
       <c r="AA32" s="9"/>
       <c r="AF32" s="9"/>
-    </row>
-    <row r="33" spans="1:32">
+      <c r="AL32" s="22"/>
+    </row>
+    <row r="33" spans="1:38">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1365,8 +1428,9 @@
       <c r="V33" s="9"/>
       <c r="AA33" s="9"/>
       <c r="AF33" s="9"/>
-    </row>
-    <row r="34" spans="1:32">
+      <c r="AL33" s="22"/>
+    </row>
+    <row r="34" spans="1:38">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1379,8 +1443,9 @@
       <c r="V34" s="9"/>
       <c r="AA34" s="9"/>
       <c r="AF34" s="9"/>
-    </row>
-    <row r="35" spans="1:32">
+      <c r="AL34" s="22"/>
+    </row>
+    <row r="35" spans="1:38">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1393,8 +1458,9 @@
       <c r="V35" s="9"/>
       <c r="AA35" s="9"/>
       <c r="AF35" s="9"/>
-    </row>
-    <row r="36" spans="1:32">
+      <c r="AL35" s="22"/>
+    </row>
+    <row r="36" spans="1:38">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1407,8 +1473,9 @@
       <c r="V36" s="9"/>
       <c r="AA36" s="9"/>
       <c r="AF36" s="9"/>
-    </row>
-    <row r="37" spans="1:32">
+      <c r="AL36" s="22"/>
+    </row>
+    <row r="37" spans="1:38">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1421,8 +1488,9 @@
       <c r="V37" s="9"/>
       <c r="AA37" s="9"/>
       <c r="AF37" s="9"/>
-    </row>
-    <row r="38" spans="1:32">
+      <c r="AL37" s="22"/>
+    </row>
+    <row r="38" spans="1:38">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1435,8 +1503,9 @@
       <c r="V38" s="9"/>
       <c r="AA38" s="9"/>
       <c r="AF38" s="9"/>
-    </row>
-    <row r="39" spans="1:32">
+      <c r="AL38" s="22"/>
+    </row>
+    <row r="39" spans="1:38">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1449,8 +1518,9 @@
       <c r="V39" s="9"/>
       <c r="AA39" s="9"/>
       <c r="AF39" s="9"/>
-    </row>
-    <row r="40" spans="1:32">
+      <c r="AL39" s="22"/>
+    </row>
+    <row r="40" spans="1:38">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1463,8 +1533,9 @@
       <c r="V40" s="9"/>
       <c r="AA40" s="9"/>
       <c r="AF40" s="9"/>
-    </row>
-    <row r="41" spans="1:32">
+      <c r="AL40" s="22"/>
+    </row>
+    <row r="41" spans="1:38">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1477,8 +1548,9 @@
       <c r="V41" s="9"/>
       <c r="AA41" s="9"/>
       <c r="AF41" s="9"/>
-    </row>
-    <row r="42" spans="1:32">
+      <c r="AL41" s="22"/>
+    </row>
+    <row r="42" spans="1:38">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1491,8 +1563,9 @@
       <c r="V42" s="9"/>
       <c r="AA42" s="9"/>
       <c r="AF42" s="9"/>
-    </row>
-    <row r="43" spans="1:32">
+      <c r="AL42" s="22"/>
+    </row>
+    <row r="43" spans="1:38">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1505,8 +1578,9 @@
       <c r="V43" s="9"/>
       <c r="AA43" s="9"/>
       <c r="AF43" s="9"/>
-    </row>
-    <row r="44" spans="1:32">
+      <c r="AL43" s="22"/>
+    </row>
+    <row r="44" spans="1:38">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1519,8 +1593,9 @@
       <c r="V44" s="9"/>
       <c r="AA44" s="9"/>
       <c r="AF44" s="9"/>
-    </row>
-    <row r="45" spans="1:32">
+      <c r="AL44" s="22"/>
+    </row>
+    <row r="45" spans="1:38">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1533,8 +1608,9 @@
       <c r="V45" s="9"/>
       <c r="AA45" s="9"/>
       <c r="AF45" s="9"/>
-    </row>
-    <row r="46" spans="1:32">
+      <c r="AL45" s="22"/>
+    </row>
+    <row r="46" spans="1:38">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1547,8 +1623,9 @@
       <c r="V46" s="9"/>
       <c r="AA46" s="9"/>
       <c r="AF46" s="9"/>
-    </row>
-    <row r="47" spans="1:32">
+      <c r="AL46" s="22"/>
+    </row>
+    <row r="47" spans="1:38">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1561,8 +1638,9 @@
       <c r="V47" s="9"/>
       <c r="AA47" s="9"/>
       <c r="AF47" s="9"/>
-    </row>
-    <row r="48" spans="1:32">
+      <c r="AL47" s="22"/>
+    </row>
+    <row r="48" spans="1:38">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1575,8 +1653,9 @@
       <c r="V48" s="9"/>
       <c r="AA48" s="9"/>
       <c r="AF48" s="9"/>
-    </row>
-    <row r="49" spans="1:35">
+      <c r="AL48" s="22"/>
+    </row>
+    <row r="49" spans="1:41">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1590,18 +1669,25 @@
       <c r="AA49" s="9"/>
       <c r="AF49" s="9"/>
       <c r="AI49" s="5"/>
-    </row>
-    <row r="50" spans="1:35">
+      <c r="AL49" s="22"/>
+    </row>
+    <row r="50" spans="1:41">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
       <c r="G50" s="9"/>
       <c r="L50" s="9"/>
       <c r="Q50" s="9"/>
       <c r="V50" s="9"/>
       <c r="AA50" s="9"/>
       <c r="AF50" s="9"/>
-    </row>
-    <row r="51" spans="1:35" s="6" customFormat="1">
+      <c r="AL50" s="22"/>
+      <c r="AM50" s="5"/>
+      <c r="AN50" s="5"/>
+    </row>
+    <row r="51" spans="1:41" s="6" customFormat="1">
       <c r="A51" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G51" s="10"/>
       <c r="L51" s="10"/>
@@ -1615,6 +1701,10 @@
       <c r="AF51" s="13"/>
       <c r="AG51" s="7"/>
       <c r="AH51" s="7"/>
+      <c r="AJ51" s="7"/>
+      <c r="AK51" s="7"/>
+      <c r="AL51" s="7"/>
+      <c r="AO51" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>